<commit_message>
CAMBIOS DEL SISTEMA, REPORTEE DE CANCELADAS, TITULOS, ETC.
</commit_message>
<xml_diff>
--- a/Presentacion/Resources/ReporteCanceladas.xlsx
+++ b/Presentacion/Resources/ReporteCanceladas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesusreyes/Desktop/Sistema-Constancias/Sistema-Constancias/Negocio/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo Perez\Documents\Contraloria\Respaldo\Sistema-Constancias\Sistema-Constancias\Presentacion\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BB70FC-319F-7642-A13C-E0ADD07D59A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A44E54-8507-41DA-891D-DB2722D50EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="4880" windowWidth="29360" windowHeight="14960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Canceladas" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>FECHA:</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Motivo de  Cancelación</t>
+  </si>
+  <si>
+    <t>Número expediente</t>
   </si>
 </sst>
 </file>
@@ -526,43 +529,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.1640625" customWidth="1"/>
+    <col min="5" max="5" width="32.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -571,20 +574,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -592,12 +595,15 @@
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>